<commit_message>
additional save to xlsx worksheet
</commit_message>
<xml_diff>
--- a/RAnalysis/Data/SDR_data/All_data_csv/Cumulative_output/Cumulative_resp_R_Analysis_worksheet.xlsx
+++ b/RAnalysis/Data/SDR_data/All_data_csv/Cumulative_output/Cumulative_resp_R_Analysis_worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samjg\Documents\Notebook\data\Geoduck_Conditioning\RAnalysis\Data\SDR_data\All_data_csv\Cumulative_output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6EBB5FF0-D8C3-41FE-9472-90EF723A1F68}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{594B79ED-7AAB-4FE5-85FA-EABDB52EE54B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12645" windowHeight="6705" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19084,7 +19084,7 @@
   <dimension ref="A1:AJ385"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A187" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N190" sqref="N190"/>
+      <selection activeCell="L190" sqref="L190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
new edits to cumulative worksheet and statistics sheets
</commit_message>
<xml_diff>
--- a/RAnalysis/Data/SDR_data/All_data_csv/Cumulative_output/Cumulative_resp_R_Analysis_worksheet.xlsx
+++ b/RAnalysis/Data/SDR_data/All_data_csv/Cumulative_output/Cumulative_resp_R_Analysis_worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samjg\Documents\Notebook\data\Geoduck_Conditioning\RAnalysis\Data\SDR_data\All_data_csv\Cumulative_output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{594B79ED-7AAB-4FE5-85FA-EABDB52EE54B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C403D89B-C644-4A91-92BB-040C0D5B1F53}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12645" windowHeight="6705" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19083,8 +19083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AJ385"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A187" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L190" sqref="L190"/>
+    <sheetView tabSelected="1" topLeftCell="A160" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L177" sqref="L177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19166,13 +19166,13 @@
         <v>20180716</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
         <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
         <v>18</v>
@@ -19184,32 +19184,32 @@
         <v>10</v>
       </c>
       <c r="H2" s="2">
-        <v>4.8880999999999997</v>
+        <v>5.1100000000000003</v>
       </c>
       <c r="I2" s="2">
-        <v>0.48520154999999998</v>
+        <v>0.78908061799999996</v>
       </c>
       <c r="J2" s="5">
-        <v>-2.8559384620000001</v>
+        <v>-2.8675057920000002</v>
       </c>
       <c r="K2" s="3">
         <f>ABS(J2)</f>
-        <v>2.8559384620000001</v>
+        <v>2.8675057920000002</v>
       </c>
       <c r="L2" s="3">
         <f>((K2))-((AVERAGE(K14:K16)))</f>
-        <v>1.8760241836666669</v>
+        <v>1.887591513666667</v>
       </c>
       <c r="M2" s="4">
         <f>(((((L2/(1000/4))*(60))*1000)/(H2*G2)))</f>
-        <v>9.2110595953437961</v>
+        <v>8.8654004555773014</v>
       </c>
       <c r="N2" s="4">
         <f>((((((L2/(1000/4))*(60))*31.998)/(H2*G2))))</f>
-        <v>0.29473548493181079</v>
+        <v>0.28367508377756251</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
@@ -19232,13 +19232,13 @@
         <v>20180716</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
         <v>18</v>
@@ -19250,32 +19250,32 @@
         <v>10</v>
       </c>
       <c r="H3" s="2">
-        <v>5.0461</v>
+        <v>4.8880999999999997</v>
       </c>
       <c r="I3" s="2">
-        <v>0.64615898500000002</v>
-      </c>
-      <c r="J3" s="1">
-        <v>-2.612595845</v>
+        <v>0.48520154999999998</v>
+      </c>
+      <c r="J3" s="5">
+        <v>-2.8559384620000001</v>
       </c>
       <c r="K3" s="3">
-        <f t="shared" ref="K3:K66" si="0">ABS(J3)</f>
-        <v>2.612595845</v>
+        <f>ABS(J3)</f>
+        <v>2.8559384620000001</v>
       </c>
       <c r="L3" s="3">
         <f>((K3))-((AVERAGE(K14:K16)))</f>
-        <v>1.6326815666666668</v>
+        <v>1.8760241836666669</v>
       </c>
       <c r="M3" s="4">
         <f>(((((L3/(1000/4))*(60))*1000)/(H3*G3)))</f>
-        <v>7.7652756782465673</v>
+        <v>9.2110595953437961</v>
       </c>
       <c r="N3" s="4">
         <f>((((((L3/(1000/4))*(60))*31.998)/(H3*G3))))</f>
-        <v>0.24847329115253367</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>180</v>
+        <v>0.29473548493181079</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
@@ -19298,13 +19298,13 @@
         <v>20180716</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
         <v>18</v>
@@ -19316,42 +19316,33 @@
         <v>10</v>
       </c>
       <c r="H4" s="2">
-        <v>5.1100000000000003</v>
+        <v>5.0461</v>
       </c>
       <c r="I4" s="2">
-        <v>0.78908061799999996</v>
-      </c>
-      <c r="J4" s="5">
-        <v>-2.8675057920000002</v>
+        <v>0.64615898500000002</v>
+      </c>
+      <c r="J4" s="1">
+        <v>-2.612595845</v>
       </c>
       <c r="K4" s="3">
-        <f t="shared" si="0"/>
-        <v>2.8675057920000002</v>
+        <f>ABS(J4)</f>
+        <v>2.612595845</v>
       </c>
       <c r="L4" s="3">
         <f>((K4))-((AVERAGE(K14:K16)))</f>
-        <v>1.887591513666667</v>
+        <v>1.6326815666666668</v>
       </c>
       <c r="M4" s="4">
         <f>(((((L4/(1000/4))*(60))*1000)/(H4*G4)))</f>
-        <v>8.8654004555773014</v>
+        <v>7.7652756782465673</v>
       </c>
       <c r="N4" s="4">
-        <f t="shared" ref="N4:N12" si="1">((((((L4/(1000/4))*(60))*31.998)/(H4*G4))))</f>
-        <v>0.28367508377756251</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
-      <c r="AA4" s="1"/>
-      <c r="AB4" s="1"/>
-      <c r="AC4" s="1"/>
-      <c r="AD4" s="1"/>
+        <f>((((((L4/(1000/4))*(60))*31.998)/(H4*G4))))</f>
+        <v>0.24847329115253367</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>180</v>
+      </c>
       <c r="AE4" s="1"/>
       <c r="AF4" s="1"/>
       <c r="AG4" s="1"/>
@@ -19391,7 +19382,7 @@
         <v>-3.8625975850000001</v>
       </c>
       <c r="K5" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="K3:K66" si="0">ABS(J5)</f>
         <v>3.8625975850000001</v>
       </c>
       <c r="L5" s="3">
@@ -19399,11 +19390,11 @@
         <v>2.6354158930000002</v>
       </c>
       <c r="M5" s="4">
-        <f t="shared" ref="M5:M12" si="2">(((((L5/(1000/4))*(60))*1000)/(H5*G5)))</f>
+        <f t="shared" ref="M5:M12" si="1">(((((L5/(1000/4))*(60))*1000)/(H5*G5)))</f>
         <v>11.608909300345056</v>
       </c>
       <c r="N5" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="N4:N12" si="2">((((((L5/(1000/4))*(60))*31.998)/(H5*G5))))</f>
         <v>0.37146187979244111</v>
       </c>
       <c r="O5" s="6" t="s">
@@ -19465,11 +19456,11 @@
         <v>2.9197722629999996</v>
       </c>
       <c r="M6" s="4">
+        <f t="shared" si="1"/>
+        <v>15.00493229523993</v>
+      </c>
+      <c r="N6" s="4">
         <f t="shared" si="2"/>
-        <v>15.00493229523993</v>
-      </c>
-      <c r="N6" s="4">
-        <f t="shared" si="1"/>
         <v>0.48012782358308737</v>
       </c>
       <c r="O6" s="6" t="s">
@@ -19531,11 +19522,11 @@
         <v>2.783983525</v>
       </c>
       <c r="M7" s="4">
+        <f t="shared" si="1"/>
+        <v>13.964137393412475</v>
+      </c>
+      <c r="N7" s="4">
         <f t="shared" si="2"/>
-        <v>13.964137393412475</v>
-      </c>
-      <c r="N7" s="4">
-        <f t="shared" si="1"/>
         <v>0.4468244683144123</v>
       </c>
       <c r="O7" s="6" t="s">
@@ -19597,11 +19588,11 @@
         <v>1.2073610039999998</v>
       </c>
       <c r="M8" s="4">
+        <f t="shared" si="1"/>
+        <v>5.8477022417583111</v>
+      </c>
+      <c r="N8" s="4">
         <f t="shared" si="2"/>
-        <v>5.8477022417583111</v>
-      </c>
-      <c r="N8" s="4">
-        <f t="shared" si="1"/>
         <v>0.18711477633178245</v>
       </c>
       <c r="O8" s="6" t="s">
@@ -19665,11 +19656,11 @@
         <v>1.0922920859999998</v>
       </c>
       <c r="M9" s="4">
+        <f t="shared" si="1"/>
+        <v>5.77126514990616</v>
+      </c>
+      <c r="N9" s="4">
         <f t="shared" si="2"/>
-        <v>5.77126514990616</v>
-      </c>
-      <c r="N9" s="4">
-        <f t="shared" si="1"/>
         <v>0.18466894226669731</v>
       </c>
       <c r="O9" s="6" t="s">
@@ -19731,11 +19722,11 @@
         <v>0.43381611899999983</v>
       </c>
       <c r="M10" s="4">
+        <f t="shared" si="1"/>
+        <v>2.1528890750811596</v>
+      </c>
+      <c r="N10" s="4">
         <f t="shared" si="2"/>
-        <v>2.1528890750811596</v>
-      </c>
-      <c r="N10" s="4">
-        <f t="shared" si="1"/>
         <v>6.8888144624446937E-2</v>
       </c>
       <c r="O10" s="6" t="s">
@@ -19799,11 +19790,11 @@
         <v>1.7471434213333337</v>
       </c>
       <c r="M11" s="4">
+        <f t="shared" si="1"/>
+        <v>8.0086027182092536</v>
+      </c>
+      <c r="N11" s="4">
         <f t="shared" si="2"/>
-        <v>8.0086027182092536</v>
-      </c>
-      <c r="N11" s="4">
-        <f t="shared" si="1"/>
         <v>0.25625926977725966</v>
       </c>
       <c r="O11" s="6" t="s">
@@ -19865,11 +19856,11 @@
         <v>0.85336219733333363</v>
       </c>
       <c r="M12" s="4">
+        <f t="shared" si="1"/>
+        <v>4.2250882402937675</v>
+      </c>
+      <c r="N12" s="4">
         <f t="shared" si="2"/>
-        <v>4.2250882402937675</v>
-      </c>
-      <c r="N12" s="4">
-        <f t="shared" si="1"/>
         <v>0.13519437351291996</v>
       </c>
       <c r="O12" s="6" t="s">
@@ -24472,15 +24463,15 @@
       </c>
       <c r="L104" s="3">
         <f>((K104))-((AVERAGE(K116:K118)))</f>
-        <v>2.5966584676666664</v>
+        <v>3.4558326793108058</v>
       </c>
       <c r="M104" s="4">
         <f t="shared" si="11"/>
-        <v>12.503973359550562</v>
+        <v>16.641248857034377</v>
       </c>
       <c r="N104" s="4">
         <f t="shared" si="10"/>
-        <v>0.40010213955889884</v>
+        <v>0.53248668092738594</v>
       </c>
       <c r="O104" s="6" t="s">
         <v>141</v>
@@ -24523,15 +24514,15 @@
       </c>
       <c r="L105" s="3">
         <f>((K105))-((AVERAGE(K116:K118)))</f>
-        <v>-7.1866595333333283E-2</v>
+        <v>0.78730761631080637</v>
       </c>
       <c r="M105" s="4">
         <f t="shared" si="11"/>
-        <v>-0.36124456247643755</v>
+        <v>3.9574797452057453</v>
       </c>
       <c r="N105" s="4">
         <f t="shared" si="10"/>
-        <v>-1.1559103510121049E-2</v>
+        <v>0.12663143688709344</v>
       </c>
       <c r="O105" s="6" t="s">
         <v>142</v>
@@ -24574,15 +24565,15 @@
       </c>
       <c r="L106" s="3">
         <f>((K106))-((AVERAGE(K116:K118)))</f>
-        <v>0.94518914866666659</v>
+        <v>1.8043633603108062</v>
       </c>
       <c r="M106" s="4">
         <f t="shared" si="11"/>
-        <v>5.0529337164597337</v>
+        <v>9.6460358997142936</v>
       </c>
       <c r="N106" s="4">
         <f t="shared" si="10"/>
-        <v>0.16168377305927856</v>
+        <v>0.30865385671905793</v>
       </c>
       <c r="O106" s="6" t="s">
         <v>143</v>
@@ -25057,12 +25048,12 @@
       <c r="I116" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="J116" s="5">
-        <v>-1.996261093</v>
+      <c r="J116" s="1">
+        <v>-0.87661195403038095</v>
       </c>
       <c r="K116" s="3">
         <f t="shared" si="7"/>
-        <v>1.996261093</v>
+        <v>0.87661195403038095</v>
       </c>
       <c r="L116" s="3" t="s">
         <v>167</v>
@@ -25105,12 +25096,12 @@
       <c r="I117" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="J117" s="5">
-        <v>-1.986152068</v>
+      <c r="J117" s="1">
+        <v>-1.32922828426482</v>
       </c>
       <c r="K117" s="3">
         <f t="shared" si="7"/>
-        <v>1.986152068</v>
+        <v>1.32922828426482</v>
       </c>
       <c r="L117" s="3" t="s">
         <v>167</v>
@@ -25153,12 +25144,12 @@
       <c r="I118" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="J118" s="5">
-        <v>-2.102115011</v>
+      <c r="J118" s="1">
+        <v>-1.3011652987723801</v>
       </c>
       <c r="K118" s="3">
         <f t="shared" si="7"/>
-        <v>2.102115011</v>
+        <v>1.3011652987723801</v>
       </c>
       <c r="L118" s="3" t="s">
         <v>167</v>

</xml_diff>

<commit_message>
a few recalculations with SDR script with criteria
</commit_message>
<xml_diff>
--- a/RAnalysis/Data/SDR_data/All_data_csv/Cumulative_output/Cumulative_resp_R_Analysis_worksheet.xlsx
+++ b/RAnalysis/Data/SDR_data/All_data_csv/Cumulative_output/Cumulative_resp_R_Analysis_worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samjg\Documents\Notebook\data\Geoduck_Conditioning\RAnalysis\Data\SDR_data\All_data_csv\Cumulative_output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C403D89B-C644-4A91-92BB-040C0D5B1F53}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{53D2C241-8735-4FB9-A774-6BF66B6949B4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12645" windowHeight="6705" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5217" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5217" uniqueCount="190">
   <si>
     <t>Date</t>
   </si>
@@ -670,6 +670,9 @@
   </si>
   <si>
     <t>Leq closest to peak density high alpha to encompass more of the jumpy data</t>
+  </si>
+  <si>
+    <t>L% - higher alpha nearest to peak density</t>
   </si>
 </sst>
 </file>
@@ -19083,8 +19086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AJ385"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L177" sqref="L177"/>
+    <sheetView tabSelected="1" topLeftCell="A139" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B155" sqref="B155:J155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19382,7 +19385,7 @@
         <v>-3.8625975850000001</v>
       </c>
       <c r="K5" s="3">
-        <f t="shared" ref="K3:K66" si="0">ABS(J5)</f>
+        <f t="shared" ref="K5:K66" si="0">ABS(J5)</f>
         <v>3.8625975850000001</v>
       </c>
       <c r="L5" s="3">
@@ -19394,7 +19397,7 @@
         <v>11.608909300345056</v>
       </c>
       <c r="N5" s="4">
-        <f t="shared" ref="N4:N12" si="2">((((((L5/(1000/4))*(60))*31.998)/(H5*G5))))</f>
+        <f t="shared" ref="N5:N12" si="2">((((((L5/(1000/4))*(60))*31.998)/(H5*G5))))</f>
         <v>0.37146187979244111</v>
       </c>
       <c r="O5" s="6" t="s">
@@ -26830,27 +26833,27 @@
       <c r="I152" s="2">
         <v>0.75042287299999999</v>
       </c>
-      <c r="J152" s="5">
-        <v>-1.9625047840000001</v>
+      <c r="J152" s="1">
+        <v>-2.2663744302334501</v>
       </c>
       <c r="K152" s="3">
         <f t="shared" si="14"/>
-        <v>1.9625047840000001</v>
+        <v>2.2663744302334501</v>
       </c>
       <c r="L152" s="3">
         <f>((K152))-((AVERAGE(K164:K166)))</f>
-        <v>1.0716366646666668</v>
+        <v>1.3755063109001169</v>
       </c>
       <c r="M152" s="4">
         <f t="shared" si="16"/>
-        <v>5.1442675318025453</v>
+        <v>6.6029585290028816</v>
       </c>
       <c r="N152" s="4">
         <f t="shared" si="15"/>
-        <v>0.16460627248261786</v>
-      </c>
-      <c r="O152" s="6" t="s">
-        <v>26</v>
+        <v>0.2112814670110342</v>
+      </c>
+      <c r="O152" s="1" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="153" spans="1:15" x14ac:dyDescent="0.25">
@@ -28273,27 +28276,27 @@
       <c r="I181" s="2">
         <v>0.61246024799999998</v>
       </c>
-      <c r="J181" s="5">
-        <v>-1.67484454</v>
+      <c r="J181" s="1">
+        <v>-3.4363858359999999</v>
       </c>
       <c r="K181" s="3">
         <f t="shared" si="14"/>
-        <v>1.67484454</v>
+        <v>3.4363858359999999</v>
       </c>
       <c r="L181" s="3">
         <f>((K181))-((AVERAGE(K191:K193)))</f>
-        <v>0.18311944599999985</v>
+        <v>1.9446607419999997</v>
       </c>
       <c r="M181" s="4">
         <f t="shared" si="18"/>
-        <v>0.84614299268386539</v>
+        <v>8.9857254154793988</v>
       </c>
       <c r="N181" s="4">
         <f t="shared" si="17"/>
-        <v>2.7074883479898327E-2</v>
-      </c>
-      <c r="O181" s="6" t="s">
-        <v>26</v>
+        <v>0.28752524184450978</v>
+      </c>
+      <c r="O181" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="182" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>